<commit_message>
Language most often fixes, boxes on mobile
</commit_message>
<xml_diff>
--- a/data-raw/variable_definitions.xlsx
+++ b/data-raw/variable_definitions.xlsx
@@ -150,13 +150,13 @@
     <t xml:space="preserve">Home language is the language spoken most often at home by a person at the time of the Census. A person can report more than one of the languages are spoken equally often.</t>
   </si>
   <si>
-    <t xml:space="preserve">English spoken at home</t>
+    <t xml:space="preserve">English spoken most often at home</t>
   </si>
   <si>
     <t xml:space="preserve">English spoken most often at home includes people who speak English most often, as well as people who speak English and other language(s) equally.</t>
   </si>
   <si>
-    <t xml:space="preserve">French spoken at home</t>
+    <t xml:space="preserve">French spoken most often at home</t>
   </si>
   <si>
     <t xml:space="preserve">French spoken most often at home includes people who speak French most often, as well as people who speak French and other language(s) equally.</t>
@@ -165,7 +165,7 @@
     <t xml:space="preserve">Non-official language spoken at home</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-official language spoken at home includes people who provided a single-response of the language spoken most often at home, which is not English or French. Shown are the top ten (if relevant) languages spoken at home.</t>
+    <t xml:space="preserve">Non-official language spoken at home includes people who provided a single-response of the language spoken most often at home, which is not English or French. Shown are the top ten (if relevant) languages most often spoken at home.</t>
   </si>
   <si>
     <t xml:space="preserve">Total household income</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">(Estimated) Median total household income</t>
   </si>
   <si>
-    <t xml:space="preserve">Median household income is the median total income for private households in 2015. If relevant, the median is estimated.</t>
+    <t xml:space="preserve">Median household income is the median total income for private households in 2015. If relevant, the median is estimated using bucket counts and assuming a uniform distribution.</t>
   </si>
   <si>
     <t xml:space="preserve">Low income (LIM-AT)</t>
@@ -344,11 +344,11 @@
   </sheetPr>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="176.81"/>

</xml_diff>

<commit_message>
Update defn to 2020
</commit_message>
<xml_diff>
--- a/data-raw/variable_definitions.xlsx
+++ b/data-raw/variable_definitions.xlsx
@@ -177,7 +177,7 @@
     <t xml:space="preserve">(Estimated) Median total household income</t>
   </si>
   <si>
-    <t xml:space="preserve">Median household income is the median total income for private households in 2015. If relevant, the median is estimated using bucket counts and assuming a uniform distribution.</t>
+    <t xml:space="preserve">Median household income is the median total income for private households in 2020. If relevant, the median is estimated using bucket counts and assuming a uniform distribution.</t>
   </si>
   <si>
     <t xml:space="preserve">Low income (LIM-AT)</t>
@@ -345,10 +345,10 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="176.81"/>

</xml_diff>

<commit_message>
Clarify 15+ for educational attainment
</commit_message>
<xml_diff>
--- a/data-raw/variable_definitions.xlsx
+++ b/data-raw/variable_definitions.xlsx
@@ -171,7 +171,7 @@
     <t xml:space="preserve">Educational attainment</t>
   </si>
   <si>
-    <t xml:space="preserve">Educational attainment refers to the highest level of education that a person has successfully completed.</t>
+    <t xml:space="preserve">Educational attainment refers to the highest level of education that a person aged 15 years and over has successfully completed.</t>
   </si>
   <si>
     <t xml:space="preserve">No high school or postsecondary</t>
@@ -365,7 +365,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add additional definitions for educational attainment
</commit_message>
<xml_diff>
--- a/data-raw/variable_definitions.xlsx
+++ b/data-raw/variable_definitions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -186,10 +186,34 @@
     <t xml:space="preserve">High school or equivalent only includes people who have this as their highest educational credential. It excludes persons with a postsecondary certificate, diploma or degree.</t>
   </si>
   <si>
-    <t xml:space="preserve">Postsecondary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postsecondary includes certificates, diplomas, and degrees from apprenticeships or trades, vocational training, CEGEP, colleges, and universities.</t>
+    <t xml:space="preserve">Apprenticeship or trades certificate or diploma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes people who have obtained a certificate, diploma or equivalent in the skilled trades or in entry-level vocations, career and technical occupations. People who also have a postsecondary certificate, diploma or degree other than an apprenticeship or trades certificate or diploma are excluded from this category.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">College, CEGEP or other non-university certificate or diploma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes people who obtained a (non-trades) postsecondary certificate or diploma of 3 months or more from a public or private college, CEGEP, polytechnic, institute of technology, school of nursing, business school or vocational school. People who also have university certificates, diplomas or degrees are also excluded from this category.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University certificate or diploma below bachelor level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes people who have obtained a university certificate or diploma below the bachelor level and who have not obtained any higher degrees, certificates or diplomas. University certificates or diplomas are commonly connected with professional associations in fields such as accounting, banking, insurance or public administration. The certificates and diplomas in this category do not require a bachelor's degree as a prerequisite.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bachelor's degree or certificate/diploma above bachelor level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes people who have obtained a bachelor's degree awarded by a degree-granting institution and people who have obtained a certificate or diploma that usually requires a bachelor's degree as a prerequisite. It excludes people who have obtained any higher degrees.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graduate or professional degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes people who have obtained degrees in medicine, dentistry, veterinary medicine or optometry; people who have obtained a master's degree; and people who have obtained a doctorate degree awarded by a university.</t>
   </si>
   <si>
     <t xml:space="preserve">Total household income</t>
@@ -362,16 +386,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6796875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="176.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="176.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -566,7 +590,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>48</v>
       </c>
@@ -574,7 +598,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>50</v>
       </c>
@@ -582,7 +606,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>52</v>
       </c>
@@ -590,7 +614,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>54</v>
       </c>
@@ -654,6 +678,42 @@
         <v>69</v>
       </c>
     </row>
+    <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>